<commit_message>
Updated non-tracing input data
</commit_message>
<xml_diff>
--- a/data/B1/Szenario-5-all21.xlsx
+++ b/data/B1/Szenario-5-all21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Friederike Mengel\Dropbox\GM_SEIR_Corona\Szenarien_04_17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friederike\Dropbox\GM_SEIR_Corona\Szenarios Discussed in Paper\B1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7107C6-89EB-40D8-B7A6-F61A907A06C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDED244C-0CF4-4342-89AE-78832FFB0157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C8D4244-D3BE-4B1B-B3FA-26E9B0BCC972}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C8D4244-D3BE-4B1B-B3FA-26E9B0BCC972}"/>
   </bookViews>
   <sheets>
     <sheet name="ideal-format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -166,7 +168,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -182,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -481,18 +483,18 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="1"/>
+    <col min="6" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -504,7 +506,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,20 +517,22 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>17041997</v>
+        <f>B16+B17+B18+B19+B20+B21+B22</f>
+        <v>17002397</v>
       </c>
       <c r="C3" s="3">
-        <v>66119010</v>
+        <f>C16+C17+C18+C19+C20+C21+C22</f>
+        <v>66000210</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +549,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,7 +566,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -579,7 +583,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -592,7 +596,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -605,7 +609,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -618,7 +622,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -631,7 +635,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -642,7 +646,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -655,7 +659,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -668,7 +672,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -681,7 +685,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -692,7 +696,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -707,7 +711,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -722,7 +726,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -737,7 +741,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -752,7 +756,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -767,7 +771,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -782,7 +786,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>